<commit_message>
Further progress toward the tutorial system and the in-game tutorial
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="220">
   <si>
     <t>key</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Crew Opinion</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
   <si>
     <t>EXCLAIMATION_MARK</t>
@@ -176,6 +182,18 @@
   </si>
   <si>
     <t>x{0}</t>
+  </si>
+  <si>
+    <t>ITALIAN</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>Language</t>
   </si>
   <si>
     <t>LOAD_GAME</t>
@@ -272,6 +290,12 @@
   </si>
   <si>
     <t>Mood</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
   <si>
     <t>MY_CREW</t>
@@ -579,6 +603,12 @@
     <t>The team captain. They'll have to be able to lead the crew and handle the pressure of doing so, all the while knowing how to react in tough situations.</t>
   </si>
   <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>Sound FX</t>
+  </si>
+  <si>
     <t>TALK_TIME_REMAINING</t>
   </si>
   <si>
@@ -639,34 +669,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>MUSIC</t>
+    <t>SHOW_TUTORIAL</t>
   </si>
   <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>SOUND</t>
-  </si>
-  <si>
-    <t>Sound FX</t>
-  </si>
-  <si>
-    <t>LANGUAGE</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>ENGLISH</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>ITALIAN</t>
-  </si>
-  <si>
-    <t>Italian</t>
+    <t>Show Tutorial:</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1064,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1078,37 +1084,37 @@
       <c r="W12" s="1"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1227,17 +1233,17 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="3" t="s">
@@ -1362,17 +1368,17 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
-      <c r="W23" s="2"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="3" t="s">
@@ -1389,17 +1395,17 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="3" t="s">
@@ -1436,7 +1442,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1456,38 +1462,38 @@
       <c r="W26" s="1"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
+      <c r="A27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
-      <c r="W27" s="2"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -1497,24 +1503,24 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
-      <c r="W28" s="2"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -1537,11 +1543,11 @@
       <c r="W29" s="1"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>60</v>
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -1551,17 +1557,17 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="3" t="s">
@@ -1605,17 +1611,17 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
-      <c r="W32" s="2"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="3" t="s">
@@ -1632,17 +1638,17 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="3" t="s">
@@ -1727,10 +1733,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -1754,10 +1760,10 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -1767,24 +1773,24 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -1794,17 +1800,17 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="3" t="s">
@@ -1902,17 +1908,17 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="3" t="s">
@@ -1983,17 +1989,17 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="3" t="s">
@@ -2050,10 +2056,10 @@
       <c r="W48" s="1"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2064,17 +2070,17 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="3" t="s">
@@ -2091,17 +2097,17 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-      <c r="W50" s="1"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="3" t="s">
@@ -2145,23 +2151,23 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="3" t="s">
+      <c r="A53" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2172,24 +2178,24 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="1"/>
-      <c r="W53" s="1"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+      <c r="V53" s="2"/>
+      <c r="W53" s="2"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>5</v>
@@ -2199,24 +2205,24 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="S54" s="2"/>
-      <c r="T54" s="2"/>
-      <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="1"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>5</v>
@@ -2240,10 +2246,10 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>5</v>
@@ -2267,10 +2273,10 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
@@ -2294,7 +2300,7 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>113</v>
@@ -2307,17 +2313,17 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
-      <c r="W58" s="1"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="2"/>
+      <c r="S58" s="2"/>
+      <c r="T58" s="2"/>
+      <c r="U58" s="2"/>
+      <c r="V58" s="2"/>
+      <c r="W58" s="2"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="3" t="s">
@@ -2326,8 +2332,8 @@
       <c r="B59" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="3">
-        <v>1.0</v>
+      <c r="C59" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
@@ -2353,25 +2359,25 @@
       <c r="B60" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="3">
-        <v>10.0</v>
+      <c r="C60" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
-      <c r="W60" s="1"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="2"/>
+      <c r="U60" s="2"/>
+      <c r="V60" s="2"/>
+      <c r="W60" s="2"/>
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="3" t="s">
@@ -2380,8 +2386,8 @@
       <c r="B61" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="3">
-        <v>2.0</v>
+      <c r="C61" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2407,8 +2413,8 @@
       <c r="B62" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C62" s="3">
-        <v>3.0</v>
+      <c r="C62" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2435,7 +2441,7 @@
         <v>123</v>
       </c>
       <c r="C63" s="3">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2462,7 +2468,7 @@
         <v>125</v>
       </c>
       <c r="C64" s="3">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2489,7 +2495,7 @@
         <v>127</v>
       </c>
       <c r="C65" s="3">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -2516,7 +2522,7 @@
         <v>129</v>
       </c>
       <c r="C66" s="3">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -2543,7 +2549,7 @@
         <v>131</v>
       </c>
       <c r="C67" s="3">
-        <v>8.0</v>
+        <v>4.0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -2570,7 +2576,7 @@
         <v>133</v>
       </c>
       <c r="C68" s="3">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2596,25 +2602,25 @@
       <c r="B69" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>5</v>
+      <c r="C69" s="3">
+        <v>6.0</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-      <c r="P69" s="2"/>
-      <c r="Q69" s="2"/>
-      <c r="R69" s="2"/>
-      <c r="S69" s="2"/>
-      <c r="T69" s="2"/>
-      <c r="U69" s="2"/>
-      <c r="V69" s="2"/>
-      <c r="W69" s="2"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3" t="s">
@@ -2623,25 +2629,25 @@
       <c r="B70" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>5</v>
+      <c r="C70" s="3">
+        <v>7.0</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
-      <c r="S70" s="2"/>
-      <c r="T70" s="2"/>
-      <c r="U70" s="2"/>
-      <c r="V70" s="2"/>
-      <c r="W70" s="2"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="3" t="s">
@@ -2650,25 +2656,25 @@
       <c r="B71" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>5</v>
+      <c r="C71" s="3">
+        <v>8.0</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-      <c r="R71" s="2"/>
-      <c r="S71" s="2"/>
-      <c r="T71" s="2"/>
-      <c r="U71" s="2"/>
-      <c r="V71" s="2"/>
-      <c r="W71" s="2"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="3" t="s">
@@ -2677,8 +2683,8 @@
       <c r="B72" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>142</v>
+      <c r="C72" s="3">
+        <v>9.0</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -2699,10 +2705,10 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>143</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>5</v>
@@ -2712,51 +2718,51 @@
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="1"/>
-      <c r="T73" s="1"/>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1"/>
-      <c r="W73" s="1"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="2"/>
+      <c r="T73" s="2"/>
+      <c r="U73" s="2"/>
+      <c r="V73" s="2"/>
+      <c r="W73" s="2"/>
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="C74" s="3" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="2"/>
+      <c r="T74" s="2"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="2"/>
+      <c r="W74" s="2"/>
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>5</v>
@@ -2766,27 +2772,27 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="1"/>
-      <c r="T75" s="1"/>
-      <c r="U75" s="1"/>
-      <c r="V75" s="1"/>
-      <c r="W75" s="1"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+      <c r="S75" s="2"/>
+      <c r="T75" s="2"/>
+      <c r="U75" s="2"/>
+      <c r="V75" s="2"/>
+      <c r="W75" s="2"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2813,7 +2819,7 @@
         <v>152</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>153</v>
+        <v>5</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2834,37 +2840,37 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="C78" s="3" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="2"/>
-      <c r="S78" s="2"/>
-      <c r="T78" s="2"/>
-      <c r="U78" s="2"/>
-      <c r="V78" s="2"/>
-      <c r="W78" s="2"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>5</v>
@@ -2887,11 +2893,11 @@
       <c r="W79" s="1"/>
     </row>
     <row r="80" ht="14.25" customHeight="1">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>5</v>
@@ -2914,14 +2920,14 @@
       <c r="W80" s="1"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="C81" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -2941,7 +2947,7 @@
       <c r="W81" s="1"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="3" t="s">
         <v>162</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -2955,17 +2961,17 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
-      <c r="M82" s="1"/>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1"/>
-      <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="1"/>
-      <c r="T82" s="1"/>
-      <c r="U82" s="1"/>
-      <c r="V82" s="1"/>
-      <c r="W82" s="1"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="2"/>
+      <c r="S82" s="2"/>
+      <c r="T82" s="2"/>
+      <c r="U82" s="2"/>
+      <c r="V82" s="2"/>
+      <c r="W82" s="2"/>
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="3" t="s">
@@ -2982,20 +2988,20 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
-      <c r="N83" s="2"/>
-      <c r="O83" s="2"/>
-      <c r="P83" s="2"/>
-      <c r="Q83" s="2"/>
-      <c r="R83" s="2"/>
-      <c r="S83" s="2"/>
-      <c r="T83" s="2"/>
-      <c r="U83" s="2"/>
-      <c r="V83" s="2"/>
-      <c r="W83" s="2"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="1"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
     </row>
     <row r="84" ht="14.25" customHeight="1">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -3022,7 +3028,7 @@
       <c r="W84" s="1"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B85" s="4" t="s">
@@ -3049,7 +3055,7 @@
       <c r="W85" s="1"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="5" t="s">
         <v>170</v>
       </c>
       <c r="B86" s="4" t="s">
@@ -3063,17 +3069,17 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="2"/>
-      <c r="S86" s="2"/>
-      <c r="T86" s="2"/>
-      <c r="U86" s="2"/>
-      <c r="V86" s="2"/>
-      <c r="W86" s="2"/>
+      <c r="M86" s="1"/>
+      <c r="N86" s="1"/>
+      <c r="O86" s="1"/>
+      <c r="P86" s="1"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="1"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="3" t="s">
@@ -3117,17 +3123,17 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="2"/>
-      <c r="Q88" s="2"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
-      <c r="T88" s="2"/>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
-      <c r="W88" s="2"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="3" t="s">
@@ -3144,17 +3150,17 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
-      <c r="M89" s="2"/>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="2"/>
-      <c r="Q89" s="2"/>
-      <c r="R89" s="2"/>
-      <c r="S89" s="2"/>
-      <c r="T89" s="2"/>
-      <c r="U89" s="2"/>
-      <c r="V89" s="2"/>
-      <c r="W89" s="2"/>
+      <c r="M89" s="1"/>
+      <c r="N89" s="1"/>
+      <c r="O89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="1"/>
+      <c r="R89" s="1"/>
+      <c r="S89" s="1"/>
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="3" t="s">
@@ -3184,10 +3190,10 @@
       <c r="W90" s="2"/>
     </row>
     <row r="91" ht="14.25" customHeight="1">
-      <c r="A91" t="s">
+      <c r="A91" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="4" t="s">
         <v>181</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3252,17 +3258,17 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
-      <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-      <c r="S93" s="1"/>
-      <c r="T93" s="1"/>
-      <c r="U93" s="1"/>
-      <c r="V93" s="1"/>
-      <c r="W93" s="1"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="2"/>
+      <c r="S93" s="2"/>
+      <c r="T93" s="2"/>
+      <c r="U93" s="2"/>
+      <c r="V93" s="2"/>
+      <c r="W93" s="2"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="3" t="s">
@@ -3279,23 +3285,23 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
-      <c r="O94" s="1"/>
-      <c r="P94" s="1"/>
-      <c r="Q94" s="1"/>
-      <c r="R94" s="1"/>
-      <c r="S94" s="1"/>
-      <c r="T94" s="1"/>
-      <c r="U94" s="1"/>
-      <c r="V94" s="1"/>
-      <c r="W94" s="1"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" s="2"/>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="2"/>
+      <c r="S94" s="2"/>
+      <c r="T94" s="2"/>
+      <c r="U94" s="2"/>
+      <c r="V94" s="2"/>
+      <c r="W94" s="2"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="3" t="s">
+      <c r="A95" t="s">
         <v>188</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>189</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -3320,10 +3326,10 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>5</v>
@@ -3333,24 +3339,24 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
-      <c r="M96" s="2"/>
-      <c r="N96" s="2"/>
-      <c r="O96" s="2"/>
-      <c r="P96" s="2"/>
-      <c r="Q96" s="2"/>
-      <c r="R96" s="2"/>
-      <c r="S96" s="2"/>
-      <c r="T96" s="2"/>
-      <c r="U96" s="2"/>
-      <c r="V96" s="2"/>
-      <c r="W96" s="2"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>5</v>
@@ -3373,11 +3379,11 @@
       <c r="W97" s="2"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" t="s">
-        <v>194</v>
+      <c r="A98" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>5</v>
@@ -3387,24 +3393,24 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
-      <c r="M98" s="2"/>
-      <c r="N98" s="2"/>
-      <c r="O98" s="2"/>
-      <c r="P98" s="2"/>
-      <c r="Q98" s="2"/>
-      <c r="R98" s="2"/>
-      <c r="S98" s="2"/>
-      <c r="T98" s="2"/>
-      <c r="U98" s="2"/>
-      <c r="V98" s="2"/>
-      <c r="W98" s="2"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="1"/>
+      <c r="S98" s="1"/>
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>5</v>
@@ -3428,10 +3434,10 @@
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>5</v>
@@ -3455,10 +3461,10 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>5</v>
@@ -3482,10 +3488,10 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>5</v>
@@ -3509,10 +3515,10 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>5</v>
@@ -3522,24 +3528,24 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-      <c r="T103" s="1"/>
-      <c r="U103" s="1"/>
-      <c r="V103" s="1"/>
-      <c r="W103" s="1"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="2"/>
+      <c r="T103" s="2"/>
+      <c r="U103" s="2"/>
+      <c r="V103" s="2"/>
+      <c r="W103" s="2"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
-      <c r="A104" s="3" t="s">
-        <v>206</v>
+      <c r="A104" t="s">
+        <v>204</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>5</v>
@@ -3563,10 +3569,10 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>5</v>
@@ -3630,17 +3636,17 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
-      <c r="M107" s="1"/>
-      <c r="N107" s="1"/>
-      <c r="O107" s="1"/>
-      <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
-      <c r="S107" s="1"/>
-      <c r="T107" s="1"/>
-      <c r="U107" s="1"/>
-      <c r="V107" s="1"/>
-      <c r="W107" s="1"/>
+      <c r="M107" s="2"/>
+      <c r="N107" s="2"/>
+      <c r="O107" s="2"/>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
+      <c r="R107" s="2"/>
+      <c r="S107" s="2"/>
+      <c r="T107" s="2"/>
+      <c r="U107" s="2"/>
+      <c r="V107" s="2"/>
+      <c r="W107" s="2"/>
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="3" t="s">
@@ -3657,17 +3663,17 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
-      <c r="M108" s="1"/>
-      <c r="N108" s="1"/>
-      <c r="O108" s="1"/>
-      <c r="P108" s="1"/>
-      <c r="Q108" s="1"/>
-      <c r="R108" s="1"/>
-      <c r="S108" s="1"/>
-      <c r="T108" s="1"/>
-      <c r="U108" s="1"/>
-      <c r="V108" s="1"/>
-      <c r="W108" s="1"/>
+      <c r="M108" s="2"/>
+      <c r="N108" s="2"/>
+      <c r="O108" s="2"/>
+      <c r="P108" s="2"/>
+      <c r="Q108" s="2"/>
+      <c r="R108" s="2"/>
+      <c r="S108" s="2"/>
+      <c r="T108" s="2"/>
+      <c r="U108" s="2"/>
+      <c r="V108" s="2"/>
+      <c r="W108" s="2"/>
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="3" t="s">
@@ -3711,20 +3717,28 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-      <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
-      <c r="S110" s="1"/>
-      <c r="T110" s="1"/>
-      <c r="U110" s="1"/>
-      <c r="V110" s="1"/>
-      <c r="W110" s="1"/>
+      <c r="M110" s="2"/>
+      <c r="N110" s="2"/>
+      <c r="O110" s="2"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="2"/>
+      <c r="S110" s="2"/>
+      <c r="T110" s="2"/>
+      <c r="U110" s="2"/>
+      <c r="V110" s="2"/>
+      <c r="W110" s="2"/>
     </row>
     <row r="111" ht="14.25" customHeight="1">
-      <c r="B111" s="1"/>
+      <c r="A111" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>

</xml_diff>

<commit_message>
Button and pop-up used to quit out of tutorial added
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="223">
   <si>
     <t>key</t>
   </si>
@@ -674,6 +674,16 @@
   <si>
     <t>Show Tutorial:</t>
   </si>
+  <si>
+    <t>TUTORIAL_WARNING</t>
+  </si>
+  <si>
+    <t>Are you sure you want to quit out of the tutorial?
+If yes, you'll need to start a new game in order to take the tutorial.</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
@@ -3757,7 +3767,15 @@
       <c r="W111" s="1"/>
     </row>
     <row r="112" ht="14.25" customHeight="1">
-      <c r="B112" s="1"/>
+      <c r="A112" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>

</xml_diff>

<commit_message>
Achievements and Leaderboard access added
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="225">
   <si>
     <t>Key</t>
   </si>
@@ -678,6 +678,18 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>ACHIEVEMENTS</t>
+  </si>
+  <si>
+    <t>Achievements</t>
+  </si>
+  <si>
+    <t>LEADERBOARDS</t>
+  </si>
+  <si>
+    <t>Leaderboards</t>
+  </si>
 </sst>
 </file>
 
@@ -3788,7 +3800,15 @@
       <c r="W112" s="3"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
-      <c r="B113" s="5"/>
+      <c r="A113" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
@@ -3807,7 +3827,15 @@
       <c r="W113" s="5"/>
     </row>
     <row r="114" ht="14.25" customHeight="1">
-      <c r="B114" s="5"/>
+      <c r="A114" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
@@ -3826,6 +3854,7 @@
       <c r="W114" s="5"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
+      <c r="A115" s="1"/>
       <c r="B115" s="5"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>

</xml_diff>

<commit_message>
Minor localization, tutorial and game loading fixes.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -28,13 +28,16 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>x</t>
+    <t>XXXX</t>
   </si>
   <si>
     <t>AGE</t>
   </si>
   <si>
     <t>Age:</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>AMPERSAND</t>
@@ -184,7 +187,7 @@
     <t>Are you sure you want to hire {0}?</t>
   </si>
   <si>
-    <t>x{0}</t>
+    <t>{0}</t>
   </si>
   <si>
     <t>ITALIAN</t>
@@ -473,7 +476,7 @@
     <t>Practice {0}/{1}</t>
   </si>
   <si>
-    <t>x{0}{1}</t>
+    <t>{0}{1}</t>
   </si>
   <si>
     <t>RACE_BUTTON_RACE</t>
@@ -507,7 +510,7 @@
     <t>{0} finished {1}!</t>
   </si>
   <si>
-    <t>{0}x{1}!</t>
+    <t>{0}{1}!</t>
   </si>
   <si>
     <t>RANDOMISE</t>
@@ -667,9 +670,6 @@
 If yes, you'll need to start a new game in order to take the tutorial.</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>WILLPOWER</t>
   </si>
   <si>
@@ -824,7 +824,7 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="3"/>
@@ -852,7 +852,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -873,13 +873,13 @@
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -900,10 +900,10 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -927,10 +927,10 @@
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -954,10 +954,10 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -981,10 +981,10 @@
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -1035,10 +1035,10 @@
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1089,10 +1089,10 @@
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>1</v>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1170,10 +1170,10 @@
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>5</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>5</v>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>5</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>5</v>
@@ -1305,10 +1305,10 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>5</v>
@@ -1332,10 +1332,10 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>5</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>5</v>
@@ -1386,10 +1386,10 @@
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>5</v>
@@ -1413,10 +1413,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>5</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>5</v>
@@ -1467,10 +1467,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>5</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
@@ -1521,13 +1521,13 @@
     </row>
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1548,13 +1548,13 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1575,10 +1575,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1602,12 +1602,12 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="3"/>
@@ -1629,10 +1629,10 @@
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>5</v>
@@ -1656,10 +1656,10 @@
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>5</v>
@@ -1683,10 +1683,10 @@
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1710,10 +1710,10 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1737,10 +1737,10 @@
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1764,10 +1764,10 @@
     </row>
     <row r="37" ht="14.25" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>5</v>
@@ -1791,10 +1791,10 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>5</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>5</v>
@@ -1845,10 +1845,10 @@
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>5</v>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>5</v>
@@ -1899,10 +1899,10 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
@@ -1926,10 +1926,10 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>5</v>
@@ -1953,10 +1953,10 @@
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>5</v>
@@ -1980,10 +1980,10 @@
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>5</v>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>5</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>5</v>
@@ -2061,10 +2061,10 @@
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>5</v>
@@ -2088,10 +2088,10 @@
     </row>
     <row r="49" ht="14.25" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>5</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>5</v>
@@ -2142,10 +2142,10 @@
     </row>
     <row r="51" ht="14.25" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>5</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="52" ht="14.25" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>5</v>
@@ -2196,10 +2196,10 @@
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>5</v>
@@ -2250,10 +2250,10 @@
     </row>
     <row r="55" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>5</v>
@@ -2277,10 +2277,10 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>5</v>
@@ -2304,10 +2304,10 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>5</v>
@@ -2331,10 +2331,10 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>5</v>
@@ -2358,10 +2358,10 @@
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>5</v>
@@ -2385,10 +2385,10 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -2412,10 +2412,10 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -2439,10 +2439,10 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -2466,10 +2466,10 @@
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>5</v>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
@@ -2520,10 +2520,10 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1">
         <v>1.0</v>
@@ -2547,10 +2547,10 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C66" s="1">
         <v>10.0</v>
@@ -2574,10 +2574,10 @@
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C67" s="1">
         <v>2.0</v>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C68" s="1">
         <v>3.0</v>
@@ -2628,10 +2628,10 @@
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C69" s="1">
         <v>4.0</v>
@@ -2655,10 +2655,10 @@
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C70" s="1">
         <v>5.0</v>
@@ -2682,10 +2682,10 @@
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C71" s="1">
         <v>6.0</v>
@@ -2709,10 +2709,10 @@
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C72" s="1">
         <v>7.0</v>
@@ -2736,10 +2736,10 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C73" s="1">
         <v>8.0</v>
@@ -2763,10 +2763,10 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C74" s="1">
         <v>9.0</v>
@@ -2790,10 +2790,10 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>5</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>5</v>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>5</v>
@@ -2871,13 +2871,13 @@
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -2898,10 +2898,10 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>5</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -2952,10 +2952,10 @@
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>5</v>
@@ -2979,10 +2979,10 @@
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>5</v>
@@ -3006,13 +3006,13 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3033,10 +3033,10 @@
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>5</v>
@@ -3060,10 +3060,10 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>5</v>
@@ -3087,10 +3087,10 @@
     </row>
     <row r="86" ht="14.25" customHeight="1">
       <c r="A86" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>5</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="87" ht="14.25" customHeight="1">
       <c r="A87" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>5</v>
@@ -3141,10 +3141,10 @@
     </row>
     <row r="88" ht="14.25" customHeight="1">
       <c r="A88" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>5</v>
@@ -3168,10 +3168,10 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>5</v>
@@ -3195,10 +3195,10 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>5</v>
@@ -3222,10 +3222,10 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>5</v>
@@ -3249,10 +3249,10 @@
     </row>
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>5</v>
@@ -3276,10 +3276,10 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>5</v>
@@ -3303,10 +3303,10 @@
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>5</v>
@@ -3330,10 +3330,10 @@
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>5</v>
@@ -3357,10 +3357,10 @@
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>5</v>
@@ -3384,10 +3384,10 @@
     </row>
     <row r="97" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>5</v>
@@ -3411,10 +3411,10 @@
     </row>
     <row r="98" ht="14.25" customHeight="1">
       <c r="A98" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>5</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>5</v>
@@ -3465,10 +3465,10 @@
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>5</v>
@@ -3492,10 +3492,10 @@
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>5</v>
@@ -3519,10 +3519,10 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>5</v>
@@ -3546,10 +3546,10 @@
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>5</v>
@@ -3573,10 +3573,10 @@
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>5</v>
@@ -3600,10 +3600,10 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>5</v>
@@ -3627,10 +3627,10 @@
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -3654,10 +3654,10 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -3681,10 +3681,10 @@
     </row>
     <row r="108" ht="14.25" customHeight="1">
       <c r="A108" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>5</v>
@@ -3708,10 +3708,10 @@
     </row>
     <row r="109" ht="14.25" customHeight="1">
       <c r="A109" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>5</v>
@@ -3735,13 +3735,13 @@
     </row>
     <row r="110" ht="14.25" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>217</v>
+        <v>5</v>
       </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>

</xml_diff>

<commit_message>
Saves now stored in 'GameSaves' sub-folder, quit to main menu warning added
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="232">
   <si>
     <t>Key</t>
   </si>
@@ -705,6 +705,12 @@
   <si>
     <t>Signed in as:</t>
   </si>
+  <si>
+    <t>MENU_QUIT_CONFIRM</t>
+  </si>
+  <si>
+    <t>Are you sure you want to quit out to the menu? Unsaved changes will be lost!</t>
+  </si>
 </sst>
 </file>
 
@@ -3923,7 +3929,15 @@
       <c r="W116" s="4"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
-      <c r="B117" s="4"/>
+      <c r="A117" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>

</xml_diff>

<commit_message>
Notification added upon boat type being changed. Reason now given for firing/hiring being disabled if the user hovers over or clicks their buttons. EventTriggers removed and replaced with event handler interfaces to improve scrolling.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="250">
   <si>
     <t>Key</t>
   </si>
@@ -125,6 +125,30 @@
   </si>
   <si>
     <t>Dismiss</t>
+  </si>
+  <si>
+    <t>FIRE_BUTTON_HOVER_ALLOWANCE</t>
+  </si>
+  <si>
+    <t>Cannot dismiss crew members due to a lack of talk time.</t>
+  </si>
+  <si>
+    <t>FIRE_BUTTON_HOVER_CREW_LIMIT</t>
+  </si>
+  <si>
+    <t>Cannot dismiss crew members as team is currently at its minimum size.</t>
+  </si>
+  <si>
+    <t>FIRE_BUTTON_HOVER_LIMIT</t>
+  </si>
+  <si>
+    <t>Cannot dismiss crew members as crew change limit ({0}) has been reached for this race session.</t>
+  </si>
+  <si>
+    <t>FIRE_BUTTON_HOVER_TUTORIAL</t>
+  </si>
+  <si>
+    <t>Cannot dismiss crew members during the tutorial.</t>
   </si>
   <si>
     <t>FIRE_WARNING</t>
@@ -284,6 +308,12 @@
   </si>
   <si>
     <t>You wanted to see me?</t>
+  </si>
+  <si>
+    <t>MENU_QUIT_CONFIRM</t>
+  </si>
+  <si>
+    <t>Are you sure you want to quit out to the menu? Unsaved changes will be lost!</t>
   </si>
   <si>
     <t>MIDBOWMAN</t>
@@ -464,6 +494,24 @@
     <t>Previous Members</t>
   </si>
   <si>
+    <t>PROMOTION_ADDED</t>
+  </si>
+  <si>
+    <t>Added</t>
+  </si>
+  <si>
+    <t>PROMOTION_HEADER</t>
+  </si>
+  <si>
+    <t>Your boat type has changed!</t>
+  </si>
+  <si>
+    <t>PROMOTION_REMOVED</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
     <t>QUICKNESS</t>
   </si>
   <si>
@@ -517,6 +565,18 @@
   </si>
   <si>
     <t>Randomise</t>
+  </si>
+  <si>
+    <t>RECRUIT_BUTTON_HOVER_ALLOWANCE</t>
+  </si>
+  <si>
+    <t>Recruitment unavilable due to lack of talk time.</t>
+  </si>
+  <si>
+    <t>RECRUIT_BUTTON_HOVER_LIMIT</t>
+  </si>
+  <si>
+    <t>Recruitment unavilable as crew change limit ({0}) has been reached for this race session.</t>
   </si>
   <si>
     <t>RECRUIT_GREETING_0</t>
@@ -603,6 +663,12 @@
     <t>Show Tutorial:</t>
   </si>
   <si>
+    <t>SIGNED_IN_AS</t>
+  </si>
+  <si>
+    <t>Signed in as:</t>
+  </si>
+  <si>
     <t>SKILLS_REQUIRED</t>
   </si>
   <si>
@@ -625,6 +691,12 @@
   </si>
   <si>
     <t>Sound FX</t>
+  </si>
+  <si>
+    <t>SUGAR_SIGN_IN</t>
+  </si>
+  <si>
+    <t>SUGAR Sign-in</t>
   </si>
   <si>
     <t>TALK_TIME_REMAINING</t>
@@ -692,24 +764,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>SUGAR_SIGN_IN</t>
-  </si>
-  <si>
-    <t>SUGAR SIGN-IN</t>
-  </si>
-  <si>
-    <t>SIGNED_IN_AS</t>
-  </si>
-  <si>
-    <t>Signed in as:</t>
-  </si>
-  <si>
-    <t>MENU_QUIT_CONFIRM</t>
-  </si>
-  <si>
-    <t>Are you sure you want to quit out to the menu? Unsaved changes will be lost!</t>
   </si>
 </sst>
 </file>
@@ -1297,17 +1351,17 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -1405,17 +1459,17 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="1" t="s">
@@ -1459,17 +1513,17 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="1" t="s">
@@ -1533,7 +1587,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1554,37 +1608,37 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>60</v>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-      <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>5</v>
@@ -1608,10 +1662,10 @@
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>5</v>
@@ -1634,65 +1688,65 @@
       <c r="W31" s="4"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="4"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>5</v>
@@ -1716,10 +1770,10 @@
     </row>
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>5</v>
@@ -1742,11 +1796,11 @@
       <c r="W35" s="4"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>72</v>
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>5</v>
@@ -1810,17 +1864,17 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="1" t="s">
@@ -1837,17 +1891,17 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="1" t="s">
@@ -1905,10 +1959,10 @@
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>5</v>
@@ -1932,10 +1986,10 @@
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>5</v>
@@ -1945,24 +1999,24 @@
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>5</v>
@@ -1972,24 +2026,24 @@
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-      <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>5</v>
@@ -2026,17 +2080,17 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
-      <c r="W46" s="4"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="1" t="s">
@@ -2107,17 +2161,17 @@
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
     </row>
     <row r="50" ht="14.25" customHeight="1">
       <c r="A50" s="1" t="s">
@@ -2188,17 +2242,17 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="4"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
       <c r="A53" s="1" t="s">
@@ -2255,10 +2309,10 @@
       <c r="W54" s="4"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2269,17 +2323,17 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="4"/>
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="1" t="s">
@@ -2323,17 +2377,17 @@
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="4"/>
-      <c r="R57" s="4"/>
-      <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
-      <c r="U57" s="4"/>
-      <c r="V57" s="4"/>
-      <c r="W57" s="4"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="1" t="s">
@@ -2350,17 +2404,17 @@
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="4"/>
     </row>
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="1" t="s">
@@ -2390,11 +2444,11 @@
       <c r="W59" s="4"/>
     </row>
     <row r="60" ht="14.25" customHeight="1">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>117</v>
+      <c r="B60" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>5</v>
@@ -2418,10 +2472,10 @@
     </row>
     <row r="61" ht="14.25" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -2445,10 +2499,10 @@
     </row>
     <row r="62" ht="14.25" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>5</v>
@@ -2458,24 +2512,24 @@
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-      <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
     </row>
     <row r="63" ht="14.25" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>5</v>
@@ -2485,24 +2539,24 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-      <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
-      <c r="U63" s="4"/>
-      <c r="V63" s="4"/>
-      <c r="W63" s="4"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
     </row>
     <row r="64" ht="14.25" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>5</v>
@@ -2526,30 +2580,30 @@
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="1">
-        <v>1.0</v>
+      <c r="C65" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-      <c r="U65" s="4"/>
-      <c r="V65" s="4"/>
-      <c r="W65" s="4"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="1" t="s">
@@ -2558,8 +2612,8 @@
       <c r="B66" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="1">
-        <v>10.0</v>
+      <c r="C66" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -2585,25 +2639,25 @@
       <c r="B67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="1">
-        <v>2.0</v>
+      <c r="C67" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="4"/>
-      <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
-      <c r="U67" s="4"/>
-      <c r="V67" s="4"/>
-      <c r="W67" s="4"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="1" t="s">
@@ -2612,8 +2666,8 @@
       <c r="B68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="1">
-        <v>3.0</v>
+      <c r="C68" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -2639,8 +2693,8 @@
       <c r="B69" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="1">
-        <v>4.0</v>
+      <c r="C69" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -2667,7 +2721,7 @@
         <v>137</v>
       </c>
       <c r="C70" s="1">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -2694,7 +2748,7 @@
         <v>139</v>
       </c>
       <c r="C71" s="1">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -2721,7 +2775,7 @@
         <v>141</v>
       </c>
       <c r="C72" s="1">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -2748,7 +2802,7 @@
         <v>143</v>
       </c>
       <c r="C73" s="1">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -2775,7 +2829,7 @@
         <v>145</v>
       </c>
       <c r="C74" s="1">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -2801,25 +2855,25 @@
       <c r="B75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>5</v>
+      <c r="C75" s="1">
+        <v>5.0</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
-      <c r="R75" s="3"/>
-      <c r="S75" s="3"/>
-      <c r="T75" s="3"/>
-      <c r="U75" s="3"/>
-      <c r="V75" s="3"/>
-      <c r="W75" s="3"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="4"/>
+      <c r="U75" s="4"/>
+      <c r="V75" s="4"/>
+      <c r="W75" s="4"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
       <c r="A76" s="1" t="s">
@@ -2828,25 +2882,25 @@
       <c r="B76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>5</v>
+      <c r="C76" s="1">
+        <v>6.0</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="3"/>
-      <c r="Q76" s="3"/>
-      <c r="R76" s="3"/>
-      <c r="S76" s="3"/>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
-      <c r="W76" s="3"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="4"/>
+      <c r="R76" s="4"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="4"/>
+      <c r="U76" s="4"/>
+      <c r="V76" s="4"/>
+      <c r="W76" s="4"/>
     </row>
     <row r="77" ht="14.25" customHeight="1">
       <c r="A77" s="1" t="s">
@@ -2855,25 +2909,25 @@
       <c r="B77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>5</v>
+      <c r="C77" s="1">
+        <v>7.0</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
-      <c r="R77" s="3"/>
-      <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
-      <c r="V77" s="3"/>
-      <c r="W77" s="3"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
     </row>
     <row r="78" ht="14.25" customHeight="1">
       <c r="A78" s="1" t="s">
@@ -2882,8 +2936,8 @@
       <c r="B78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>154</v>
+      <c r="C78" s="1">
+        <v>8.0</v>
       </c>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
@@ -2904,13 +2958,13 @@
     </row>
     <row r="79" ht="14.25" customHeight="1">
       <c r="A79" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>5</v>
+      <c r="C79" s="1">
+        <v>9.0</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -2931,37 +2985,37 @@
     </row>
     <row r="80" ht="14.25" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="C80" s="1" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="4"/>
-      <c r="R80" s="4"/>
-      <c r="S80" s="4"/>
-      <c r="T80" s="4"/>
-      <c r="U80" s="4"/>
-      <c r="V80" s="4"/>
-      <c r="W80" s="4"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
     </row>
     <row r="81" ht="14.25" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>5</v>
@@ -2971,24 +3025,24 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4"/>
-      <c r="U81" s="4"/>
-      <c r="V81" s="4"/>
-      <c r="W81" s="4"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
     </row>
     <row r="82" ht="14.25" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>5</v>
@@ -3012,13 +3066,13 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="C83" s="1" t="s">
-        <v>165</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3039,10 +3093,10 @@
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>5</v>
@@ -3052,24 +3106,24 @@
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
-      <c r="P84" s="3"/>
-      <c r="Q84" s="3"/>
-      <c r="R84" s="3"/>
-      <c r="S84" s="3"/>
-      <c r="T84" s="3"/>
-      <c r="U84" s="3"/>
-      <c r="V84" s="3"/>
-      <c r="W84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="4"/>
+      <c r="U84" s="4"/>
+      <c r="V84" s="4"/>
+      <c r="W84" s="4"/>
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>5</v>
@@ -3079,27 +3133,27 @@
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="4"/>
-      <c r="R85" s="4"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="4"/>
-      <c r="U85" s="4"/>
-      <c r="V85" s="4"/>
-      <c r="W85" s="4"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
@@ -3119,11 +3173,11 @@
       <c r="W86" s="4"/>
     </row>
     <row r="87" ht="14.25" customHeight="1">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>172</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>5</v>
@@ -3146,14 +3200,14 @@
       <c r="W87" s="4"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="C88" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3174,10 +3228,10 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>5</v>
@@ -3187,24 +3241,24 @@
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="3"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
-      <c r="Q89" s="3"/>
-      <c r="R89" s="3"/>
-      <c r="S89" s="3"/>
-      <c r="T89" s="3"/>
-      <c r="U89" s="3"/>
-      <c r="V89" s="3"/>
-      <c r="W89" s="3"/>
+      <c r="M89" s="4"/>
+      <c r="N89" s="4"/>
+      <c r="O89" s="4"/>
+      <c r="P89" s="4"/>
+      <c r="Q89" s="4"/>
+      <c r="R89" s="4"/>
+      <c r="S89" s="4"/>
+      <c r="T89" s="4"/>
+      <c r="U89" s="4"/>
+      <c r="V89" s="4"/>
+      <c r="W89" s="4"/>
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>5</v>
@@ -3228,13 +3282,13 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3295,17 +3349,17 @@
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="N93" s="3"/>
-      <c r="O93" s="3"/>
-      <c r="P93" s="3"/>
-      <c r="Q93" s="3"/>
-      <c r="R93" s="3"/>
-      <c r="S93" s="3"/>
-      <c r="T93" s="3"/>
-      <c r="U93" s="3"/>
-      <c r="V93" s="3"/>
-      <c r="W93" s="3"/>
+      <c r="M93" s="4"/>
+      <c r="N93" s="4"/>
+      <c r="O93" s="4"/>
+      <c r="P93" s="4"/>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="4"/>
+      <c r="S93" s="4"/>
+      <c r="T93" s="4"/>
+      <c r="U93" s="4"/>
+      <c r="V93" s="4"/>
+      <c r="W93" s="4"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
       <c r="A94" s="1" t="s">
@@ -3322,17 +3376,17 @@
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="3"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-      <c r="Q94" s="3"/>
-      <c r="R94" s="3"/>
-      <c r="S94" s="3"/>
-      <c r="T94" s="3"/>
-      <c r="U94" s="3"/>
-      <c r="V94" s="3"/>
-      <c r="W94" s="3"/>
+      <c r="M94" s="4"/>
+      <c r="N94" s="4"/>
+      <c r="O94" s="4"/>
+      <c r="P94" s="4"/>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
+      <c r="S94" s="4"/>
+      <c r="T94" s="4"/>
+      <c r="U94" s="4"/>
+      <c r="V94" s="4"/>
+      <c r="W94" s="4"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
       <c r="A95" s="1" t="s">
@@ -3349,20 +3403,20 @@
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="3"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-      <c r="Q95" s="3"/>
-      <c r="R95" s="3"/>
-      <c r="S95" s="3"/>
-      <c r="T95" s="3"/>
-      <c r="U95" s="3"/>
-      <c r="V95" s="3"/>
-      <c r="W95" s="3"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
+      <c r="S95" s="4"/>
+      <c r="T95" s="4"/>
+      <c r="U95" s="4"/>
+      <c r="V95" s="4"/>
+      <c r="W95" s="4"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="5" t="s">
         <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
@@ -3376,23 +3430,23 @@
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
-      <c r="S96" s="3"/>
-      <c r="T96" s="3"/>
-      <c r="U96" s="3"/>
-      <c r="V96" s="3"/>
-      <c r="W96" s="3"/>
+      <c r="M96" s="4"/>
+      <c r="N96" s="4"/>
+      <c r="O96" s="4"/>
+      <c r="P96" s="4"/>
+      <c r="Q96" s="4"/>
+      <c r="R96" s="4"/>
+      <c r="S96" s="4"/>
+      <c r="T96" s="4"/>
+      <c r="U96" s="4"/>
+      <c r="V96" s="4"/>
+      <c r="W96" s="4"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" t="s">
+      <c r="A97" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -3403,24 +3457,24 @@
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
-      <c r="R97" s="3"/>
-      <c r="S97" s="3"/>
-      <c r="T97" s="3"/>
-      <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
-      <c r="W97" s="3"/>
+      <c r="M97" s="4"/>
+      <c r="N97" s="4"/>
+      <c r="O97" s="4"/>
+      <c r="P97" s="4"/>
+      <c r="Q97" s="4"/>
+      <c r="R97" s="4"/>
+      <c r="S97" s="4"/>
+      <c r="T97" s="4"/>
+      <c r="U97" s="4"/>
+      <c r="V97" s="4"/>
+      <c r="W97" s="4"/>
     </row>
     <row r="98" ht="14.25" customHeight="1">
-      <c r="A98" s="1" t="s">
-        <v>192</v>
+      <c r="A98" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>5</v>
@@ -3444,10 +3498,10 @@
     </row>
     <row r="99" ht="14.25" customHeight="1">
       <c r="A99" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>5</v>
@@ -3457,24 +3511,24 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="4"/>
-      <c r="T99" s="4"/>
-      <c r="U99" s="4"/>
-      <c r="V99" s="4"/>
-      <c r="W99" s="4"/>
+      <c r="M99" s="3"/>
+      <c r="N99" s="3"/>
+      <c r="O99" s="3"/>
+      <c r="P99" s="3"/>
+      <c r="Q99" s="3"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="3"/>
+      <c r="T99" s="3"/>
+      <c r="U99" s="3"/>
+      <c r="V99" s="3"/>
+      <c r="W99" s="3"/>
     </row>
     <row r="100" ht="14.25" customHeight="1">
       <c r="A100" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>5</v>
@@ -3484,24 +3538,24 @@
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-      <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
-      <c r="S100" s="3"/>
-      <c r="T100" s="3"/>
-      <c r="U100" s="3"/>
-      <c r="V100" s="3"/>
-      <c r="W100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="4"/>
+      <c r="Q100" s="4"/>
+      <c r="R100" s="4"/>
+      <c r="S100" s="4"/>
+      <c r="T100" s="4"/>
+      <c r="U100" s="4"/>
+      <c r="V100" s="4"/>
+      <c r="W100" s="4"/>
     </row>
     <row r="101" ht="14.25" customHeight="1">
       <c r="A101" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>5</v>
@@ -3525,10 +3579,10 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>5</v>
@@ -3538,24 +3592,24 @@
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="4"/>
-      <c r="P102" s="4"/>
-      <c r="Q102" s="4"/>
-      <c r="R102" s="4"/>
-      <c r="S102" s="4"/>
-      <c r="T102" s="4"/>
-      <c r="U102" s="4"/>
-      <c r="V102" s="4"/>
-      <c r="W102" s="4"/>
+      <c r="M102" s="3"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="3"/>
+      <c r="P102" s="3"/>
+      <c r="Q102" s="3"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="3"/>
+      <c r="T102" s="3"/>
+      <c r="U102" s="3"/>
+      <c r="V102" s="3"/>
+      <c r="W102" s="3"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>5</v>
@@ -3565,24 +3619,24 @@
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="4"/>
-      <c r="R103" s="4"/>
-      <c r="S103" s="4"/>
-      <c r="T103" s="4"/>
-      <c r="U103" s="4"/>
-      <c r="V103" s="4"/>
-      <c r="W103" s="4"/>
+      <c r="M103" s="3"/>
+      <c r="N103" s="3"/>
+      <c r="O103" s="3"/>
+      <c r="P103" s="3"/>
+      <c r="Q103" s="3"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="3"/>
+      <c r="T103" s="3"/>
+      <c r="U103" s="3"/>
+      <c r="V103" s="3"/>
+      <c r="W103" s="3"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>5</v>
@@ -3606,10 +3660,10 @@
     </row>
     <row r="105" ht="14.25" customHeight="1">
       <c r="A105" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>5</v>
@@ -3633,10 +3687,10 @@
     </row>
     <row r="106" ht="14.25" customHeight="1">
       <c r="A106" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -3660,10 +3714,10 @@
     </row>
     <row r="107" ht="14.25" customHeight="1">
       <c r="A107" t="s">
-        <v>210</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -3808,17 +3862,17 @@
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
-      <c r="M112" s="3"/>
-      <c r="N112" s="3"/>
-      <c r="O112" s="3"/>
-      <c r="P112" s="3"/>
-      <c r="Q112" s="3"/>
-      <c r="R112" s="3"/>
-      <c r="S112" s="3"/>
-      <c r="T112" s="3"/>
-      <c r="U112" s="3"/>
-      <c r="V112" s="3"/>
-      <c r="W112" s="3"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+      <c r="U112" s="4"/>
+      <c r="V112" s="4"/>
+      <c r="W112" s="4"/>
     </row>
     <row r="113" ht="14.25" customHeight="1">
       <c r="A113" s="1" t="s">
@@ -3862,17 +3916,17 @@
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
-      <c r="M114" s="3"/>
-      <c r="N114" s="3"/>
-      <c r="O114" s="3"/>
-      <c r="P114" s="3"/>
-      <c r="Q114" s="3"/>
-      <c r="R114" s="3"/>
-      <c r="S114" s="3"/>
-      <c r="T114" s="3"/>
-      <c r="U114" s="3"/>
-      <c r="V114" s="3"/>
-      <c r="W114" s="3"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4"/>
+      <c r="W114" s="4"/>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="1" t="s">
@@ -3916,17 +3970,17 @@
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
-      <c r="M116" s="4"/>
-      <c r="N116" s="4"/>
-      <c r="O116" s="4"/>
-      <c r="P116" s="4"/>
-      <c r="Q116" s="4"/>
-      <c r="R116" s="4"/>
-      <c r="S116" s="4"/>
-      <c r="T116" s="4"/>
-      <c r="U116" s="4"/>
-      <c r="V116" s="4"/>
-      <c r="W116" s="4"/>
+      <c r="M116" s="3"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="3"/>
+      <c r="P116" s="3"/>
+      <c r="Q116" s="3"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="3"/>
+      <c r="T116" s="3"/>
+      <c r="U116" s="3"/>
+      <c r="V116" s="3"/>
+      <c r="W116" s="3"/>
     </row>
     <row r="117" ht="14.25" customHeight="1">
       <c r="A117" s="1" t="s">
@@ -3943,58 +3997,82 @@
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
-      <c r="O117" s="4"/>
-      <c r="P117" s="4"/>
-      <c r="Q117" s="4"/>
-      <c r="R117" s="4"/>
-      <c r="S117" s="4"/>
-      <c r="T117" s="4"/>
-      <c r="U117" s="4"/>
-      <c r="V117" s="4"/>
-      <c r="W117" s="4"/>
+      <c r="M117" s="3"/>
+      <c r="N117" s="3"/>
+      <c r="O117" s="3"/>
+      <c r="P117" s="3"/>
+      <c r="Q117" s="3"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="3"/>
+      <c r="T117" s="3"/>
+      <c r="U117" s="3"/>
+      <c r="V117" s="3"/>
+      <c r="W117" s="3"/>
     </row>
     <row r="118" ht="14.25" customHeight="1">
-      <c r="B118" s="4"/>
+      <c r="A118" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
-      <c r="M118" s="4"/>
-      <c r="N118" s="4"/>
-      <c r="O118" s="4"/>
-      <c r="P118" s="4"/>
-      <c r="Q118" s="4"/>
-      <c r="R118" s="4"/>
-      <c r="S118" s="4"/>
-      <c r="T118" s="4"/>
-      <c r="U118" s="4"/>
-      <c r="V118" s="4"/>
-      <c r="W118" s="4"/>
+      <c r="M118" s="3"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="3"/>
+      <c r="P118" s="3"/>
+      <c r="Q118" s="3"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="3"/>
+      <c r="T118" s="3"/>
+      <c r="U118" s="3"/>
+      <c r="V118" s="3"/>
+      <c r="W118" s="3"/>
     </row>
     <row r="119" ht="14.25" customHeight="1">
-      <c r="B119" s="4"/>
+      <c r="A119" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
-      <c r="M119" s="4"/>
-      <c r="N119" s="4"/>
-      <c r="O119" s="4"/>
-      <c r="P119" s="4"/>
-      <c r="Q119" s="4"/>
-      <c r="R119" s="4"/>
-      <c r="S119" s="4"/>
-      <c r="T119" s="4"/>
-      <c r="U119" s="4"/>
-      <c r="V119" s="4"/>
-      <c r="W119" s="4"/>
+      <c r="M119" s="3"/>
+      <c r="N119" s="3"/>
+      <c r="O119" s="3"/>
+      <c r="P119" s="3"/>
+      <c r="Q119" s="3"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="3"/>
+      <c r="T119" s="3"/>
+      <c r="U119" s="3"/>
+      <c r="V119" s="3"/>
+      <c r="W119" s="3"/>
     </row>
     <row r="120" ht="14.25" customHeight="1">
-      <c r="B120" s="4"/>
+      <c r="A120" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
@@ -4013,7 +4091,15 @@
       <c r="W120" s="4"/>
     </row>
     <row r="121" ht="14.25" customHeight="1">
-      <c r="B121" s="4"/>
+      <c r="A121" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
@@ -4032,7 +4118,15 @@
       <c r="W121" s="4"/>
     </row>
     <row r="122" ht="14.25" customHeight="1">
-      <c r="B122" s="4"/>
+      <c r="A122" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
@@ -4051,45 +4145,69 @@
       <c r="W122" s="4"/>
     </row>
     <row r="123" ht="14.25" customHeight="1">
-      <c r="B123" s="4"/>
+      <c r="A123" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
-      <c r="M123" s="4"/>
-      <c r="N123" s="4"/>
-      <c r="O123" s="4"/>
-      <c r="P123" s="4"/>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
-      <c r="S123" s="4"/>
-      <c r="T123" s="4"/>
-      <c r="U123" s="4"/>
-      <c r="V123" s="4"/>
-      <c r="W123" s="4"/>
+      <c r="M123" s="3"/>
+      <c r="N123" s="3"/>
+      <c r="O123" s="3"/>
+      <c r="P123" s="3"/>
+      <c r="Q123" s="3"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="3"/>
+      <c r="T123" s="3"/>
+      <c r="U123" s="3"/>
+      <c r="V123" s="3"/>
+      <c r="W123" s="3"/>
     </row>
     <row r="124" ht="14.25" customHeight="1">
-      <c r="B124" s="4"/>
+      <c r="A124" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="4"/>
-      <c r="O124" s="4"/>
-      <c r="P124" s="4"/>
-      <c r="Q124" s="4"/>
-      <c r="R124" s="4"/>
-      <c r="S124" s="4"/>
-      <c r="T124" s="4"/>
-      <c r="U124" s="4"/>
-      <c r="V124" s="4"/>
-      <c r="W124" s="4"/>
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="3"/>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="3"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="3"/>
+      <c r="T124" s="3"/>
+      <c r="U124" s="3"/>
+      <c r="V124" s="3"/>
+      <c r="W124" s="3"/>
     </row>
     <row r="125" ht="14.25" customHeight="1">
-      <c r="B125" s="4"/>
+      <c r="A125" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
@@ -4108,23 +4226,31 @@
       <c r="W125" s="4"/>
     </row>
     <row r="126" ht="14.25" customHeight="1">
-      <c r="B126" s="4"/>
+      <c r="A126" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
-      <c r="M126" s="4"/>
-      <c r="N126" s="4"/>
-      <c r="O126" s="4"/>
-      <c r="P126" s="4"/>
-      <c r="Q126" s="4"/>
-      <c r="R126" s="4"/>
-      <c r="S126" s="4"/>
-      <c r="T126" s="4"/>
-      <c r="U126" s="4"/>
-      <c r="V126" s="4"/>
-      <c r="W126" s="4"/>
+      <c r="M126" s="3"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+      <c r="P126" s="3"/>
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="3"/>
+      <c r="T126" s="3"/>
+      <c r="U126" s="3"/>
+      <c r="V126" s="3"/>
+      <c r="W126" s="3"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
       <c r="B127" s="4"/>

</xml_diff>

<commit_message>
Scrollbar sensitivity adjusted, warning now displayed if the same line-up is used two race sessions in a row
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Localization.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="252">
   <si>
     <t>Key</t>
   </si>
@@ -765,6 +765,12 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>REPEAT_CONFIRM</t>
+  </si>
+  <si>
+    <t>Are you sure you want to use the same crew line-up as the previous race?</t>
+  </si>
 </sst>
 </file>
 
@@ -4253,7 +4259,15 @@
       <c r="W126" s="3"/>
     </row>
     <row r="127" ht="14.25" customHeight="1">
-      <c r="B127" s="4"/>
+      <c r="A127" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>

</xml_diff>